<commit_message>
Grimstone Beasts 번역 갱신
</commit_message>
<xml_diff>
--- a/Data/Grimstone Beasts - 3309790710/3309790710.xlsx
+++ b/Data/Grimstone Beasts - 3309790710/3309790710.xlsx
@@ -1,26 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bjmi0\Desktop\림월드 번역\Grimstone Beasts - 3309790710\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\SteamLibrary\steamapps\common\RimWorld\Mods\RMK\Data\Grimstone Beasts - 3309790710\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7230930-C958-4657-A13C-DD980FE54B87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60FA3B88-9128-496F-849E-01A96BB8D19F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="691" uniqueCount="489">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="496">
   <si>
     <t>Class+Node [(Identifier (Key)]</t>
   </si>
@@ -1551,6 +1564,27 @@
   <si>
     <t>몸통</t>
     <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>머리</t>
+  </si>
+  <si>
+    <t>ThingDef+Grimstone_NorthernLynx.tools.0.label</t>
+  </si>
+  <si>
+    <t>Grimstone_NorthernLynx.tools.0.label</t>
+  </si>
+  <si>
+    <t>ThingDef+Grimstone_NorthernLynx.tools.1.label</t>
+  </si>
+  <si>
+    <t>Grimstone_NorthernLynx.tools.1.label</t>
+  </si>
+  <si>
+    <t>ThingDef+Grimstone_NorthernLynx.tools.3.label</t>
+  </si>
+  <si>
+    <t>Grimstone_NorthernLynx.tools.3.label</t>
   </si>
 </sst>
 </file>
@@ -1597,10 +1631,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -1903,19 +1936,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F138"/>
+  <dimension ref="A1:F141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G76" sqref="G76"/>
+      <selection activeCell="L141" sqref="L141"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="17" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="7" width="9.1796875" style="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.1796875" style="1"/>
+    <col min="1" max="7" width="9.140625" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1935,7 +1968,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
@@ -1952,7 +1985,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>10</v>
       </c>
@@ -1969,7 +2002,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -1986,7 +2019,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -2003,7 +2036,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>20</v>
       </c>
@@ -2020,7 +2053,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>23</v>
       </c>
@@ -2037,7 +2070,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>26</v>
       </c>
@@ -2054,7 +2087,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>29</v>
       </c>
@@ -2071,7 +2104,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -2088,7 +2121,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>35</v>
       </c>
@@ -2105,7 +2138,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>38</v>
       </c>
@@ -2122,7 +2155,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
         <v>41</v>
       </c>
@@ -2139,7 +2172,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
         <v>44</v>
       </c>
@@ -2156,7 +2189,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
         <v>47</v>
       </c>
@@ -2173,7 +2206,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>50</v>
       </c>
@@ -2190,7 +2223,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
         <v>53</v>
       </c>
@@ -2207,7 +2240,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>56</v>
       </c>
@@ -2224,7 +2257,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
         <v>59</v>
       </c>
@@ -2241,7 +2274,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
         <v>62</v>
       </c>
@@ -2258,7 +2291,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
         <v>66</v>
       </c>
@@ -2275,7 +2308,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
         <v>69</v>
       </c>
@@ -2292,7 +2325,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
         <v>71</v>
       </c>
@@ -2309,7 +2342,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
         <v>73</v>
       </c>
@@ -2326,7 +2359,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
         <v>75</v>
       </c>
@@ -2343,7 +2376,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
         <v>77</v>
       </c>
@@ -2360,7 +2393,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
         <v>79</v>
       </c>
@@ -2377,7 +2410,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>81</v>
       </c>
@@ -2394,7 +2427,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>84</v>
       </c>
@@ -2411,7 +2444,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>87</v>
       </c>
@@ -2428,7 +2461,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>89</v>
       </c>
@@ -2445,7 +2478,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="s">
         <v>91</v>
       </c>
@@ -2462,7 +2495,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
         <v>94</v>
       </c>
@@ -2479,7 +2512,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="s">
         <v>97</v>
       </c>
@@ -2496,7 +2529,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="s">
         <v>99</v>
       </c>
@@ -2513,7 +2546,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="s">
         <v>101</v>
       </c>
@@ -2530,7 +2563,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="s">
         <v>104</v>
       </c>
@@ -2547,7 +2580,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>106</v>
       </c>
@@ -2564,7 +2597,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
         <v>109</v>
       </c>
@@ -2581,7 +2614,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="s">
         <v>112</v>
       </c>
@@ -2598,7 +2631,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="1" t="s">
         <v>115</v>
       </c>
@@ -2615,7 +2648,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="s">
         <v>118</v>
       </c>
@@ -2632,7 +2665,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="s">
         <v>121</v>
       </c>
@@ -2649,7 +2682,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
         <v>124</v>
       </c>
@@ -2666,7 +2699,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="s">
         <v>127</v>
       </c>
@@ -2683,7 +2716,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="s">
         <v>130</v>
       </c>
@@ -2700,7 +2733,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="s">
         <v>133</v>
       </c>
@@ -2717,7 +2750,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="s">
         <v>136</v>
       </c>
@@ -2734,7 +2767,7 @@
         <v>421</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="s">
         <v>139</v>
       </c>
@@ -2751,7 +2784,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>141</v>
       </c>
@@ -2768,7 +2801,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="s">
         <v>143</v>
       </c>
@@ -2785,7 +2818,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="s">
         <v>145</v>
       </c>
@@ -2802,7 +2835,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
         <v>147</v>
       </c>
@@ -2819,7 +2852,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="s">
         <v>149</v>
       </c>
@@ -2836,7 +2869,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="s">
         <v>153</v>
       </c>
@@ -2853,7 +2886,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="s">
         <v>156</v>
       </c>
@@ -2870,7 +2903,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="s">
         <v>159</v>
       </c>
@@ -2887,7 +2920,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="s">
         <v>162</v>
       </c>
@@ -2904,7 +2937,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="s">
         <v>165</v>
       </c>
@@ -2921,7 +2954,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="s">
         <v>168</v>
       </c>
@@ -2938,7 +2971,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="1" t="s">
         <v>172</v>
       </c>
@@ -2955,7 +2988,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="s">
         <v>175</v>
       </c>
@@ -2972,7 +3005,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="s">
         <v>178</v>
       </c>
@@ -2989,7 +3022,7 @@
         <v>474</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="s">
         <v>181</v>
       </c>
@@ -3006,7 +3039,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>184</v>
       </c>
@@ -3023,7 +3056,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="s">
         <v>187</v>
       </c>
@@ -3040,7 +3073,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="s">
         <v>190</v>
       </c>
@@ -3057,7 +3090,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="s">
         <v>193</v>
       </c>
@@ -3074,7 +3107,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="s">
         <v>196</v>
       </c>
@@ -3091,7 +3124,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
         <v>199</v>
       </c>
@@ -3108,7 +3141,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
         <v>202</v>
       </c>
@@ -3125,7 +3158,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
         <v>205</v>
       </c>
@@ -3142,7 +3175,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="s">
         <v>208</v>
       </c>
@@ -3159,7 +3192,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="s">
         <v>211</v>
       </c>
@@ -3176,7 +3209,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="s">
         <v>214</v>
       </c>
@@ -3193,7 +3226,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>217</v>
       </c>
@@ -3210,7 +3243,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="s">
         <v>220</v>
       </c>
@@ -3227,7 +3260,7 @@
         <v>486</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="s">
         <v>223</v>
       </c>
@@ -3244,7 +3277,7 @@
         <v>487</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="s">
         <v>226</v>
       </c>
@@ -3261,7 +3294,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="s">
         <v>229</v>
       </c>
@@ -3278,7 +3311,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="s">
         <v>232</v>
       </c>
@@ -3295,7 +3328,7 @@
         <v>473</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
         <v>235</v>
       </c>
@@ -3312,7 +3345,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="s">
         <v>237</v>
       </c>
@@ -3329,7 +3362,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
         <v>240</v>
       </c>
@@ -3346,7 +3379,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
         <v>243</v>
       </c>
@@ -3363,7 +3396,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
         <v>246</v>
       </c>
@@ -3380,7 +3413,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="1" t="s">
         <v>249</v>
       </c>
@@ -3397,7 +3430,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="s">
         <v>252</v>
       </c>
@@ -3414,7 +3447,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
         <v>254</v>
       </c>
@@ -3431,7 +3464,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="s">
         <v>257</v>
       </c>
@@ -3448,7 +3481,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="s">
         <v>259</v>
       </c>
@@ -3465,7 +3498,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="s">
         <v>262</v>
       </c>
@@ -3482,7 +3515,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="1" t="s">
         <v>265</v>
       </c>
@@ -3499,7 +3532,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
         <v>267</v>
       </c>
@@ -3516,7 +3549,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
         <v>270</v>
       </c>
@@ -3533,7 +3566,7 @@
         <v>462</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="s">
         <v>273</v>
       </c>
@@ -3550,7 +3583,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="s">
         <v>276</v>
       </c>
@@ -3567,7 +3600,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
         <v>279</v>
       </c>
@@ -3584,7 +3617,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="s">
         <v>281</v>
       </c>
@@ -3601,7 +3634,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
         <v>282</v>
       </c>
@@ -3618,7 +3651,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="s">
         <v>285</v>
       </c>
@@ -3635,7 +3668,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="s">
         <v>288</v>
       </c>
@@ -3652,7 +3685,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="s">
         <v>291</v>
       </c>
@@ -3669,7 +3702,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="s">
         <v>294</v>
       </c>
@@ -3686,7 +3719,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="s">
         <v>296</v>
       </c>
@@ -3703,7 +3736,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
         <v>298</v>
       </c>
@@ -3720,7 +3753,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="s">
         <v>299</v>
       </c>
@@ -3737,7 +3770,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="s">
         <v>302</v>
       </c>
@@ -3754,7 +3787,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="s">
         <v>305</v>
       </c>
@@ -3771,7 +3804,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="s">
         <v>308</v>
       </c>
@@ -3784,11 +3817,11 @@
       <c r="E110" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="F110" s="2" t="s">
+      <c r="F110" s="1" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
         <v>311</v>
       </c>
@@ -3805,7 +3838,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="s">
         <v>314</v>
       </c>
@@ -3822,7 +3855,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="s">
         <v>317</v>
       </c>
@@ -3839,7 +3872,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="s">
         <v>319</v>
       </c>
@@ -3856,7 +3889,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="s">
         <v>321</v>
       </c>
@@ -3873,7 +3906,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="s">
         <v>323</v>
       </c>
@@ -3890,7 +3923,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="s">
         <v>325</v>
       </c>
@@ -3907,7 +3940,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="s">
         <v>326</v>
       </c>
@@ -3924,7 +3957,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="s">
         <v>329</v>
       </c>
@@ -3941,7 +3974,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
         <v>332</v>
       </c>
@@ -3958,7 +3991,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
         <v>335</v>
       </c>
@@ -3975,7 +4008,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
         <v>338</v>
       </c>
@@ -3992,7 +4025,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
         <v>339</v>
       </c>
@@ -4009,7 +4042,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
         <v>342</v>
       </c>
@@ -4026,7 +4059,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
         <v>345</v>
       </c>
@@ -4043,7 +4076,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="s">
         <v>348</v>
       </c>
@@ -4060,7 +4093,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>350</v>
       </c>
@@ -4077,7 +4110,7 @@
         <v>426</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="s">
         <v>352</v>
       </c>
@@ -4094,7 +4127,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="s">
         <v>354</v>
       </c>
@@ -4111,7 +4144,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="s">
         <v>355</v>
       </c>
@@ -4128,7 +4161,7 @@
         <v>431</v>
       </c>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="s">
         <v>358</v>
       </c>
@@ -4145,7 +4178,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="s">
         <v>361</v>
       </c>
@@ -4162,7 +4195,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="s">
         <v>364</v>
       </c>
@@ -4175,11 +4208,11 @@
       <c r="E133" s="1" t="s">
         <v>366</v>
       </c>
-      <c r="F133" s="2" t="s">
+      <c r="F133" s="1" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="s">
         <v>367</v>
       </c>
@@ -4196,7 +4229,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="s">
         <v>369</v>
       </c>
@@ -4213,7 +4246,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="s">
         <v>371</v>
       </c>
@@ -4230,7 +4263,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="s">
         <v>373</v>
       </c>
@@ -4247,7 +4280,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="s">
         <v>374</v>
       </c>
@@ -4262,6 +4295,48 @@
       </c>
       <c r="F138" s="1" t="s">
         <v>435</v>
+      </c>
+    </row>
+    <row r="139" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A139" s="1" t="s">
+        <v>490</v>
+      </c>
+      <c r="B139" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>491</v>
+      </c>
+      <c r="F139" s="1" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A140" s="1" t="s">
+        <v>492</v>
+      </c>
+      <c r="B140" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C140" s="1" t="s">
+        <v>493</v>
+      </c>
+      <c r="F140" s="1" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A141" s="1" t="s">
+        <v>494</v>
+      </c>
+      <c r="B141" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C141" s="1" t="s">
+        <v>495</v>
+      </c>
+      <c r="F141" s="1" t="s">
+        <v>489</v>
       </c>
     </row>
   </sheetData>

</xml_diff>